<commit_message>
Started work on generating case and advocate data from journals (1955-1962 so far)
</commit_message>
<xml_diff>
--- a/sources/ld/women-advocates.xlsx
+++ b/sources/ld/women-advocates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/Sites/loners/lonedissent/sources/ld/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648E0381-100D-7F47-8EDC-0A60384BA52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710BB47F-6A7B-A649-84EA-0193DE159CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="1040" windowWidth="27460" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7760" yWindow="-19620" windowWidth="27460" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="women-advocates" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5415" uniqueCount="3798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5440" uniqueCount="3808">
   <si>
     <t>nameAdvocate</t>
   </si>
@@ -11414,6 +11414,36 @@
   </si>
   <si>
     <t>https://www.supremecourt.gov/oral_arguments/argument_transcripts/2023/23-3_1b72.pdf</t>
+  </si>
+  <si>
+    <t>Dallas, Texas</t>
+  </si>
+  <si>
+    <t>No. 22-1079. Truck Insurance Exchange v. Kaiser Gypsum Company, Inc.</t>
+  </si>
+  <si>
+    <t>https://www.supremecourt.gov/oral_arguments/argument_transcripts/2023/22-1079_o7kq.pdf</t>
+  </si>
+  <si>
+    <t>Anya A. Bidwell</t>
+  </si>
+  <si>
+    <t>Arlington, Virginia</t>
+  </si>
+  <si>
+    <t>No. 22-1025. Sylvia Gonzalez v. Edward Trevino</t>
+  </si>
+  <si>
+    <t>https://www.supremecourt.gov/oral_arguments/argument_transcripts/2023/22-1025_m6io.pdf</t>
+  </si>
+  <si>
+    <t>on behalf of Texas</t>
+  </si>
+  <si>
+    <t>https://www.supremecourt.gov/oral_arguments/argument_transcripts/2023/141-orig_2_g314.pdf</t>
+  </si>
+  <si>
+    <t>Principal Deputy Solicitor General, Austin, Texas</t>
   </si>
 </sst>
 </file>
@@ -12280,11 +12310,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1661"/>
+  <dimension ref="A1:H1666"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1638" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1660" sqref="A1660"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36749,6 +36779,106 @@
         <v>3797</v>
       </c>
     </row>
+    <row r="1662" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1662" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>3798</v>
+      </c>
+      <c r="C1662" s="2">
+        <v>45370</v>
+      </c>
+      <c r="D1662" t="s">
+        <v>3799</v>
+      </c>
+      <c r="F1662" s="6" t="s">
+        <v>3664</v>
+      </c>
+      <c r="G1662" s="6" t="s">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1663" t="s">
+        <v>3801</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>3802</v>
+      </c>
+      <c r="C1663" s="2">
+        <v>45371</v>
+      </c>
+      <c r="D1663" t="s">
+        <v>3803</v>
+      </c>
+      <c r="F1663" s="6" t="s">
+        <v>3664</v>
+      </c>
+      <c r="G1663" s="6" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1664" t="s">
+        <v>3510</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>3417</v>
+      </c>
+      <c r="C1664" s="2">
+        <v>45371</v>
+      </c>
+      <c r="D1664" t="s">
+        <v>3803</v>
+      </c>
+      <c r="F1664" s="6" t="s">
+        <v>3718</v>
+      </c>
+      <c r="G1664" s="6" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1665" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1665" s="2">
+        <v>45371</v>
+      </c>
+      <c r="D1665" t="s">
+        <v>3803</v>
+      </c>
+      <c r="F1665" s="6" t="s">
+        <v>3640</v>
+      </c>
+      <c r="G1665" s="6" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1666" t="s">
+        <v>3499</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>3807</v>
+      </c>
+      <c r="C1666" s="2">
+        <v>45371</v>
+      </c>
+      <c r="D1666" t="s">
+        <v>3341</v>
+      </c>
+      <c r="F1666" s="6" t="s">
+        <v>3805</v>
+      </c>
+      <c r="G1666" s="6" t="s">
+        <v>3806</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>